<commit_message>
actualizar guías de implementación
</commit_message>
<xml_diff>
--- a/fhir/ig/r2bo/0.1.1-ballot/StructureDefinition-r2bo-composition-biopsia.xlsx
+++ b/fhir/ig/r2bo/0.1.1-ballot/StructureDefinition-r2bo-composition-biopsia.xlsx
@@ -45,7 +45,7 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Perfil del Documento de Biopsía</t>
+    <t>Perfil de la Cabecera del Documento de Biopsía</t>
   </si>
   <si>
     <t>Status</t>
@@ -63,7 +63,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-12-12T16:54:01-03:00</t>
+    <t>2025-12-23T17:10:55-03:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>